<commit_message>
updated financial calculations with latest work progress
git-svn-id: svn://localhost/ARK/trunk@8247 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/TestFilesAndDocuments/steering committee/NeCTAR/NeCTAR Reporting/Reporting Financial Calculations.xlsx
+++ b/usefulTools/TestFilesAndDocuments/steering committee/NeCTAR/NeCTAR Reporting/Reporting Financial Calculations.xlsx
@@ -183,15 +183,6 @@
     <t>Dec-March</t>
   </si>
   <si>
-    <t>March-May</t>
-  </si>
-  <si>
-    <t>May-August</t>
-  </si>
-  <si>
-    <t>Aug-Nov</t>
-  </si>
-  <si>
     <t>Cumulative</t>
   </si>
   <si>
@@ -398,6 +389,15 @@
   </si>
   <si>
     <t>total combined?</t>
+  </si>
+  <si>
+    <t>March-June</t>
+  </si>
+  <si>
+    <t>July-Sep</t>
+  </si>
+  <si>
+    <t>Sep - Dec</t>
   </si>
 </sst>
 </file>
@@ -1878,45 +1878,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="59" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="59" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1970,6 +1931,45 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="59" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="59" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5245,7 +5245,7 @@
   <sheetData>
     <row r="1" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B1" s="121" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C1" s="134" t="str">
         <f>OVERALLLIGHT</f>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="2" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B2" s="121" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" s="131" t="str">
         <f>MILESTONELIGHT</f>
@@ -5265,7 +5265,7 @@
     </row>
     <row r="3" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B3" s="121" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="131" t="str">
         <f>ISSUELIGHT</f>
@@ -5275,7 +5275,7 @@
     </row>
     <row r="4" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B4" s="121" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C4" s="131" t="str">
         <f>RISKLIGHT</f>
@@ -5285,7 +5285,7 @@
     </row>
     <row r="5" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B5" s="121" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C5" s="131" t="str">
         <f>CHANGELIGHT</f>
@@ -5295,7 +5295,7 @@
     </row>
     <row r="6" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B6" s="121" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C6" s="132" t="str">
         <f>DEPENDENCYLIGHT</f>
@@ -5305,7 +5305,7 @@
     </row>
     <row r="7" spans="2:13" s="27" customFormat="1" ht="12.75">
       <c r="B7" s="121" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C7" s="132" t="str">
         <f>MEASURELIGHT</f>
@@ -5315,7 +5315,7 @@
     </row>
     <row r="8" spans="2:13" s="27" customFormat="1">
       <c r="B8" s="121" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" s="131" t="str">
         <f>COMMUNICATIONLIGHT</f>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="9" spans="2:13" s="27" customFormat="1">
       <c r="B9" s="121" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C9" s="130" t="str">
         <f>FINANCELIGHT</f>
@@ -5354,7 +5354,7 @@
     <row r="12" spans="2:13" s="27" customFormat="1" ht="15.95" customHeight="1">
       <c r="B12" s="121"/>
       <c r="C12" s="125" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D12" s="124">
         <f>ReportFrom</f>
@@ -5365,7 +5365,7 @@
     <row r="13" spans="2:13" s="27" customFormat="1" ht="15.95" customHeight="1">
       <c r="B13" s="121"/>
       <c r="C13" s="123" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D13" s="122">
         <f>LastDateReport</f>
@@ -5382,13 +5382,13 @@
     </row>
     <row r="15" spans="2:13" s="27" customFormat="1" ht="18.95" customHeight="1">
       <c r="C15" s="117" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D15" s="117"/>
       <c r="E15" s="117"/>
       <c r="F15" s="117"/>
       <c r="I15" s="117" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J15" s="117" t="str">
         <f>FINANCELIGHT</f>
@@ -5425,18 +5425,18 @@
       <c r="B18" s="28"/>
       <c r="C18" s="116"/>
       <c r="D18" s="115"/>
-      <c r="E18" s="142" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
+      <c r="E18" s="159" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="160"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="161"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="145" t="s">
-        <v>83</v>
-      </c>
-      <c r="K18" s="146"/>
-      <c r="L18" s="147"/>
+      <c r="J18" s="162" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="163"/>
+      <c r="L18" s="164"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
       <c r="O18" s="28"/>
@@ -5451,32 +5451,32 @@
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="114" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="113" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F19" s="112" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G19" s="112" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" s="111" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I19" s="110" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J19" s="109" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K19" s="108" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L19" s="107" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
@@ -5550,109 +5550,109 @@
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O22" s="28"/>
       <c r="P22" s="28"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="28"/>
       <c r="S22" s="97" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T22" s="97" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="U22" s="96"/>
     </row>
     <row r="23" spans="1:21" s="87" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="148" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="150" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="151"/>
-      <c r="D23" s="135" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="138" t="s">
+      <c r="A23" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="135"/>
-      <c r="G23" s="135"/>
-      <c r="H23" s="139"/>
-      <c r="I23" s="140" t="s">
+      <c r="B23" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="J23" s="160" t="s">
+      <c r="C23" s="138"/>
+      <c r="D23" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="161"/>
-      <c r="L23" s="162"/>
-      <c r="M23" s="163" t="s">
+      <c r="E23" s="155" t="s">
         <v>64</v>
       </c>
+      <c r="F23" s="153"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="156"/>
+      <c r="I23" s="157" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="147" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="148"/>
+      <c r="L23" s="149"/>
+      <c r="M23" s="150" t="s">
+        <v>61</v>
+      </c>
       <c r="N23" s="89"/>
-      <c r="P23" s="137" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q23" s="137" t="s">
-        <v>62</v>
+      <c r="P23" s="152" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q23" s="152" t="s">
+        <v>59</v>
       </c>
       <c r="S23" s="95" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="T23" s="94" t="str">
         <f>IF(I38&lt;&gt;I39,"RED","Correct "&amp;I38&amp;" = "&amp;I39)</f>
         <v>Correct 289000 = 289000</v>
       </c>
-      <c r="U23" s="152" t="s">
-        <v>60</v>
+      <c r="U23" s="139" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="87" customFormat="1" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A24" s="149"/>
+      <c r="A24" s="136"/>
       <c r="B24" s="93" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="136"/>
+        <v>55</v>
+      </c>
+      <c r="D24" s="154"/>
       <c r="E24" s="92" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F24" s="91" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G24" s="91" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H24" s="90" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="141"/>
+        <v>42</v>
+      </c>
+      <c r="I24" s="158"/>
       <c r="J24" s="92" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K24" s="91" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L24" s="90" t="s">
-        <v>45</v>
-      </c>
-      <c r="M24" s="164"/>
+        <v>42</v>
+      </c>
+      <c r="M24" s="151"/>
       <c r="N24" s="89"/>
-      <c r="P24" s="137"/>
-      <c r="Q24" s="137"/>
+      <c r="P24" s="152"/>
+      <c r="Q24" s="152"/>
       <c r="S24" s="87" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T24" s="88">
         <f>I39*0.3</f>
         <v>86700</v>
       </c>
-      <c r="U24" s="153"/>
+      <c r="U24" s="140"/>
     </row>
     <row r="25" spans="1:21" s="27" customFormat="1" ht="15.75" customHeight="1">
       <c r="A25" s="71">
@@ -5775,7 +5775,7 @@
       </c>
       <c r="R26" s="28"/>
       <c r="S26" s="28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="T26" s="28">
         <f>LASTQUARTER</f>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="R27" s="28"/>
       <c r="S27" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T27" s="39">
         <f>I39*0.2</f>
@@ -5953,7 +5953,7 @@
       </c>
       <c r="R29" s="28"/>
       <c r="S29" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="T29" s="28" t="str">
         <f>IF(T23="RED","RED",IF(T25="RED","RED",IF(T28="AMBER","AMBER","GREEN")))</f>
@@ -6398,7 +6398,7 @@
       <c r="A38" s="28"/>
       <c r="B38" s="51"/>
       <c r="C38" s="50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D38" s="49">
         <f t="shared" ref="D38:M38" si="8">SUM(D25:D37)</f>
@@ -6464,7 +6464,7 @@
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I39" s="40">
         <f>E20</f>
@@ -6512,16 +6512,16 @@
       <c r="C41" s="28"/>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
-      <c r="F41" s="157" t="str">
+      <c r="F41" s="144" t="str">
         <f>IF(N25&gt;"",N25,IF(N26&gt;"",N26,IF(N27&gt;"",N27,IF(N28&gt;"",N28,IF(N29&gt;"",N29,IF(N30&gt;"",N30,IF(N31&gt;"",N31,IF(N32&gt;"",N32,IF(N33&gt;"",N33,IF(N34&gt;"",N34,IF(N35&gt;"",N35,IF(N36&gt;"",N36,IF(N37&gt;"",N37,IF(I38&lt;&gt;I39,"Your total estimate in cell I38 does not yet equal the Nectar Funds Allocated",""))))))))))))))</f>
         <v/>
       </c>
-      <c r="G41" s="158"/>
-      <c r="H41" s="158"/>
-      <c r="I41" s="158"/>
-      <c r="J41" s="158"/>
-      <c r="K41" s="158"/>
-      <c r="L41" s="159"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
+      <c r="K41" s="145"/>
+      <c r="L41" s="146"/>
       <c r="M41" s="28"/>
       <c r="N41" s="28"/>
       <c r="O41" s="28"/>
@@ -6536,7 +6536,7 @@
       <c r="A42" s="28"/>
       <c r="B42" s="28"/>
       <c r="C42" s="38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D42" s="37"/>
       <c r="E42" s="28"/>
@@ -6560,17 +6560,17 @@
     <row r="43" spans="1:21" s="27" customFormat="1" ht="54" customHeight="1" thickBot="1">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
-      <c r="C43" s="154"/>
-      <c r="D43" s="155"/>
-      <c r="E43" s="155"/>
-      <c r="F43" s="155"/>
-      <c r="G43" s="155"/>
-      <c r="H43" s="155"/>
-      <c r="I43" s="155"/>
-      <c r="J43" s="155"/>
-      <c r="K43" s="155"/>
-      <c r="L43" s="155"/>
-      <c r="M43" s="156"/>
+      <c r="C43" s="141"/>
+      <c r="D43" s="142"/>
+      <c r="E43" s="142"/>
+      <c r="F43" s="142"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="142"/>
+      <c r="I43" s="142"/>
+      <c r="J43" s="142"/>
+      <c r="K43" s="142"/>
+      <c r="L43" s="142"/>
+      <c r="M43" s="143"/>
       <c r="N43" s="28"/>
       <c r="O43" s="28"/>
       <c r="P43" s="28"/>
@@ -6638,7 +6638,7 @@
         <v>42369</v>
       </c>
       <c r="R45" s="34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="S45" s="28"/>
       <c r="T45" s="28"/>
@@ -6648,7 +6648,7 @@
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D46" s="33"/>
       <c r="E46" s="32">
@@ -6702,7 +6702,7 @@
       <c r="A47" s="28"/>
       <c r="B47" s="28"/>
       <c r="C47" s="30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="29">
@@ -6769,7 +6769,7 @@
       <c r="A48" s="28"/>
       <c r="B48" s="28"/>
       <c r="C48" s="30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="29">
@@ -6834,7 +6834,7 @@
     </row>
     <row r="49" spans="3:18" s="27" customFormat="1" ht="12.75" hidden="1">
       <c r="C49" s="30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="29">
@@ -6896,7 +6896,7 @@
     </row>
     <row r="50" spans="3:18" s="27" customFormat="1" ht="12.75" hidden="1">
       <c r="C50" s="30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="29">
@@ -6958,7 +6958,7 @@
     </row>
     <row r="51" spans="3:18" s="27" customFormat="1" ht="15" hidden="1" customHeight="1">
       <c r="C51" s="30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="29">
@@ -7020,7 +7020,7 @@
     </row>
     <row r="52" spans="3:18" s="27" customFormat="1" ht="25.5" hidden="1">
       <c r="C52" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D52" s="33"/>
       <c r="E52" s="32">
@@ -7069,7 +7069,7 @@
     </row>
     <row r="53" spans="3:18" s="27" customFormat="1" ht="12.75" hidden="1">
       <c r="C53" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D53" s="30"/>
       <c r="E53" s="29">
@@ -7131,7 +7131,7 @@
     </row>
     <row r="54" spans="3:18" s="27" customFormat="1" ht="12.75" hidden="1">
       <c r="C54" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="29">
@@ -7193,7 +7193,7 @@
     </row>
     <row r="55" spans="3:18" s="27" customFormat="1" ht="12.75" hidden="1">
       <c r="C55" s="30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D55" s="30"/>
       <c r="E55" s="29">
@@ -7255,7 +7255,7 @@
     </row>
     <row r="56" spans="3:18" s="27" customFormat="1" ht="12.75" hidden="1">
       <c r="C56" s="30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="29">
@@ -7336,6 +7336,8 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
   <mergeCells count="14">
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="J18:L18"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="U23:U24"/>
@@ -7348,8 +7350,6 @@
     <mergeCell ref="P23:P24"/>
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="I23:I24"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="J18:L18"/>
   </mergeCells>
   <conditionalFormatting sqref="C1">
     <cfRule type="cellIs" dxfId="165" priority="164" operator="equal">
@@ -8210,22 +8210,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="0.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="61.5" thickBot="1">
@@ -8255,17 +8263,17 @@
       <c r="K1" s="165"/>
       <c r="L1" s="22"/>
       <c r="M1" s="165" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="N1" s="165"/>
       <c r="O1" s="22"/>
       <c r="P1" s="165" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="Q1" s="165"/>
       <c r="R1" s="22"/>
       <c r="S1" s="165" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="T1" s="165"/>
     </row>
@@ -8308,34 +8316,34 @@
       </c>
       <c r="E3" s="13"/>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1">
@@ -8819,26 +8827,26 @@
         <v>0</v>
       </c>
       <c r="L11" s="24">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M11" s="11">
         <f t="shared" si="1"/>
-        <v>44100</v>
+        <v>29400</v>
       </c>
       <c r="N11" s="11">
         <f t="shared" si="0"/>
-        <v>8733.75</v>
+        <v>5822.5</v>
       </c>
       <c r="O11" s="24">
         <v>1</v>
       </c>
       <c r="P11" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14700</v>
       </c>
       <c r="Q11" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2911.25</v>
       </c>
       <c r="R11" s="24">
         <v>1</v>
@@ -8932,26 +8940,26 @@
         <v>1856</v>
       </c>
       <c r="L13" s="23">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="M13" s="11">
         <f t="shared" si="1"/>
-        <v>9371.25</v>
+        <v>18742.5</v>
       </c>
       <c r="N13" s="11">
         <f>($L13-$I13)*E13</f>
-        <v>1856</v>
+        <v>3712</v>
       </c>
       <c r="O13" s="24">
         <v>1</v>
       </c>
       <c r="P13" s="11">
         <f t="shared" si="2"/>
-        <v>9371.25</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="11">
         <f>($O13-$L13)*E13</f>
-        <v>1856</v>
+        <v>0</v>
       </c>
       <c r="R13" s="24">
         <v>1</v>
@@ -9076,26 +9084,26 @@
         <v>0</v>
       </c>
       <c r="L15" s="21">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="M15" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17151.25</v>
       </c>
       <c r="N15" s="11">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4927</v>
       </c>
       <c r="O15" s="23">
         <v>0.75</v>
       </c>
       <c r="P15" s="11">
         <f t="shared" si="2"/>
-        <v>51453.75</v>
+        <v>34302.5</v>
       </c>
       <c r="Q15" s="11">
         <f>($O15-$L15)*E15</f>
-        <v>14781</v>
+        <v>9854</v>
       </c>
       <c r="R15" s="23">
         <v>1</v>
@@ -9122,7 +9130,7 @@
       </c>
       <c r="E16" s="15"/>
       <c r="S16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" thickBot="1">
@@ -9207,19 +9215,19 @@
       </c>
       <c r="M21" s="11">
         <f>SUM(M4:M15)</f>
-        <v>60141.25</v>
+        <v>71963.75</v>
       </c>
       <c r="N21" s="11">
         <f>SUM(N4:N15)</f>
-        <v>10944.75</v>
+        <v>14816.5</v>
       </c>
       <c r="P21" s="11">
         <f>SUM(P4:P15)</f>
-        <v>60825</v>
+        <v>49002.5</v>
       </c>
       <c r="Q21" s="11">
         <f>SUM(Q4:Q15)</f>
-        <v>16637</v>
+        <v>12765.25</v>
       </c>
       <c r="S21" s="11">
         <f>SUM(S4:S15)</f>
@@ -9232,7 +9240,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="F22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J22" s="11">
         <f>G21+J21</f>
@@ -9244,11 +9252,11 @@
       </c>
       <c r="M22" s="11">
         <f>M21+J22</f>
-        <v>212622.75</v>
+        <v>224445.25</v>
       </c>
       <c r="N22" s="11">
         <f>N21+K22</f>
-        <v>95693</v>
+        <v>99564.75</v>
       </c>
       <c r="P22" s="11">
         <f>P21+M22</f>
@@ -9269,7 +9277,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="F23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H23" s="11">
         <f>G21+H21</f>
@@ -9284,8 +9292,8 @@
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11">
-        <f t="shared" ref="L23:T23" si="11">M22+N22</f>
-        <v>308315.75</v>
+        <f t="shared" ref="N23:T23" si="11">M22+N22</f>
+        <v>324010</v>
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>

</xml_diff>